<commit_message>
cargar asignatura y usuarios
</commit_message>
<xml_diff>
--- a/public/formatos/plantilla_docente_asignaturas_clases.xlsx
+++ b/public/formatos/plantilla_docente_asignaturas_clases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29022"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29429"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{7DB991F5-215A-4182-8DB6-A24BAFFF2565}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{4601E151-E917-458C-990B-D221A5B57973}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="asignaturas_y_clases" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>codigoAsignatura</t>
   </si>
@@ -39,13 +39,13 @@
     <t>nombreAsignatura</t>
   </si>
   <si>
-    <t>fechaClase (YYYY-MM-DD)</t>
-  </si>
-  <si>
-    <t>horaInicio (HH:MM)</t>
-  </si>
-  <si>
-    <t>horaFin (HH:MM)</t>
+    <t>fechaClase (MM/DD/YYYY)</t>
+  </si>
+  <si>
+    <t>horaInicio (HH:MM:SS AM o PM)</t>
+  </si>
+  <si>
+    <t>horaFin (HH:MM:SS AM o PM)</t>
   </si>
   <si>
     <t>temaClase</t>
@@ -63,19 +63,10 @@
     <t>semestreAsignatura</t>
   </si>
   <si>
-    <t>ASIG001</t>
-  </si>
-  <si>
-    <t>Matemáticas Básicas</t>
-  </si>
-  <si>
-    <t>2025-08-01</t>
-  </si>
-  <si>
-    <t>08:00</t>
-  </si>
-  <si>
-    <t>10:00</t>
+    <t>MAT003</t>
+  </si>
+  <si>
+    <t>Matematicas II</t>
   </si>
   <si>
     <t>Introducción</t>
@@ -91,13 +82,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Liberation Sans"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -120,17 +117,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="19" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -153,44 +150,44 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="1F497D"/>
+        <a:srgbClr val="0E2841"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="EEECE1"/>
+        <a:srgbClr val="E8E8E8"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4F81BD"/>
+        <a:srgbClr val="145F82"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="C0504D"/>
+        <a:srgbClr val="E87331"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="9BBB59"/>
+        <a:srgbClr val="186C24"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="8064A2"/>
+        <a:srgbClr val="0F9ED5"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="4BACC6"/>
+        <a:srgbClr val="A02B93"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="F79646"/>
+        <a:srgbClr val="4EA72E"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0000FF"/>
+        <a:srgbClr val="467886"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="800080"/>
+        <a:srgbClr val="96607D"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线 Light"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
@@ -217,14 +214,32 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
         <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hans" typeface="等线"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Arial"/>
         <a:font script="Hebr" typeface="Arial"/>
@@ -251,6 +266,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -262,166 +295,162 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
+            <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="63000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
+          <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults/>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
   <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
 </a:theme>
 </file>
 
@@ -430,49 +459,49 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="27.140625" customWidth="1"/>
-    <col min="3" max="3" width="31.28515625" customWidth="1"/>
-    <col min="4" max="4" width="25.42578125" customWidth="1"/>
-    <col min="5" max="5" width="18.7109375" customWidth="1"/>
-    <col min="6" max="6" width="23.140625" customWidth="1"/>
-    <col min="7" max="7" width="30.140625" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="9" width="25.5703125" customWidth="1"/>
-    <col min="10" max="10" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="33.140625" customWidth="1"/>
+    <col min="2" max="2" width="28.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.7109375" customWidth="1"/>
+    <col min="4" max="4" width="32.5703125" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" customWidth="1"/>
+    <col min="6" max="6" width="21.28515625" customWidth="1"/>
+    <col min="7" max="7" width="24" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" customWidth="1"/>
+    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="10" max="10" width="22.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="21.75" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:10">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="1" t="s">
@@ -480,38 +509,38 @@
       </c>
     </row>
     <row r="2" spans="1:10">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2">
+        <v>45957</v>
+      </c>
+      <c r="D2" s="3">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E2" s="3">
+        <v>0.70833333333333337</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="G2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" s="1">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" t="s">
-        <v>16</v>
-      </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
-        <v>17</v>
-      </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>6</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>